<commit_message>
gsb as not a NB marker
</commit_message>
<xml_diff>
--- a/Stablestates/25Oct_S1model.xlsx
+++ b/Stablestates/25Oct_S1model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybahar/Documents/Git/DevelopmentalSignaling/Stablestates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED71AD-87B5-2744-B437-D62FCCB7ABE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13851C38-55DB-F14F-9A16-187E841CACF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="980" windowWidth="25100" windowHeight="19040" activeTab="6" xr2:uid="{10AF4D6B-B7E4-5644-8352-3E93EADC3131}"/>
+    <workbookView xWindow="14140" yWindow="2680" windowWidth="25100" windowHeight="19040" activeTab="6" xr2:uid="{10AF4D6B-B7E4-5644-8352-3E93EADC3131}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="57">
   <si>
     <t>Intermediate</t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t xml:space="preserve">EGFR </t>
+  </si>
+  <si>
+    <t>NB7-4</t>
+  </si>
+  <si>
+    <t>NB7-1</t>
+  </si>
+  <si>
+    <t>NB5-6</t>
+  </si>
+  <si>
+    <t>NB5-3</t>
+  </si>
+  <si>
+    <t>NB5-2</t>
   </si>
 </sst>
 </file>
@@ -53103,7 +53118,7 @@
   <dimension ref="A1:AL41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54402,7 +54417,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C14" s="42">
         <v>0</v>
@@ -54508,7 +54523,7 @@
     <row r="15" spans="1:38" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="72"/>
       <c r="B15" s="73" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C15" s="29">
         <v>0</v>
@@ -54614,7 +54629,7 @@
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="72"/>
       <c r="B16" s="73" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C16" s="29">
         <v>0</v>
@@ -54720,7 +54735,7 @@
     <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="72"/>
       <c r="B17" s="73" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C17" s="29">
         <v>0</v>
@@ -54826,7 +54841,7 @@
     <row r="18" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="72"/>
       <c r="B18" s="73" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C18" s="31">
         <v>0</v>

</xml_diff>